<commit_message>
video - libro campo - dpf
</commit_message>
<xml_diff>
--- a/files/data.xlsx
+++ b/files/data.xlsx
@@ -17,16 +17,16 @@
     <t xml:space="preserve">bar_code</t>
   </si>
   <si>
-    <t xml:space="preserve">ID</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Block</t>
-  </si>
-  <si>
-    <t xml:space="preserve">IBTH</t>
-  </si>
-  <si>
-    <t xml:space="preserve">IBT</t>
+    <t xml:space="preserve">plots</t>
+  </si>
+  <si>
+    <t xml:space="preserve">block</t>
+  </si>
+  <si>
+    <t xml:space="preserve">imb</t>
+  </si>
+  <si>
+    <t xml:space="preserve">imbt</t>
   </si>
   <si>
     <t xml:space="preserve">PE2015_101_I_8</t>

</xml_diff>